<commit_message>
Mensaje descriptivo de los cambios
</commit_message>
<xml_diff>
--- a/cypress/fixtures/datos.xlsx
+++ b/cypress/fixtures/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Cypress\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD227916-058B-4545-9112-24B0B4C69FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D6C58-8D3E-4F23-9877-F065DFC5BE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>APELLIDO2</t>
   </si>
   <si>
-    <t>ENF-777-179</t>
-  </si>
-  <si>
     <t>MED-777-180</t>
+  </si>
+  <si>
+    <t>ENF-777-555</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +439,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Revisión por pares y actualización
</commit_message>
<xml_diff>
--- a/cypress/fixtures/datos.xlsx
+++ b/cypress/fixtures/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NSEM\Automatizaci-n\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA95B3A-9053-4CB5-9272-738D54FC878C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7545E0C-C49E-471D-A1AF-F3A0F2295F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>DNI</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Cruz</t>
   </si>
   <si>
-    <t>Olvera</t>
-  </si>
-  <si>
     <t>01-02-1985</t>
   </si>
   <si>
@@ -57,32 +54,78 @@
     <t>APELLIDO2</t>
   </si>
   <si>
-    <t>AUT_QA_CY_002</t>
-  </si>
-  <si>
-    <t>AUT_QA_CY_003</t>
-  </si>
-  <si>
-    <t>Felipe</t>
-  </si>
-  <si>
-    <t>Caty</t>
+    <t>AUT_ODON_001</t>
+  </si>
+  <si>
+    <t>AUT_ODON_002</t>
+  </si>
+  <si>
+    <t>AUT_PSIC_001</t>
+  </si>
+  <si>
+    <t>AUT_PSIC_002</t>
+  </si>
+  <si>
+    <t>AUT_NUTRI_001</t>
+  </si>
+  <si>
+    <t>AUT_NUTRI_002</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Gibran</t>
+  </si>
+  <si>
+    <t>Pedraza</t>
+  </si>
+  <si>
+    <t>Morroy</t>
+  </si>
+  <si>
+    <t>Kaarina</t>
+  </si>
+  <si>
+    <t>Jiménez</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Cerro</t>
+  </si>
+  <si>
+    <t>Marlenne</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>Gónzales</t>
+  </si>
+  <si>
+    <t>Nancy</t>
+  </si>
+  <si>
+    <t>Meza</t>
+  </si>
+  <si>
+    <t>Zuñiga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,9 +153,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -394,15 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -419,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -427,43 +469,105 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>